<commit_message>
added methods to calculate opportunity cost of leaving VTSAX. updated driver.py
</commit_message>
<xml_diff>
--- a/src/crsr_data/CRSRTrackingGrid.xlsx
+++ b/src/crsr_data/CRSRTrackingGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/src/crsr_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA4B0B-2634-434A-8A3A-7694173B226F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0080B1F8-DDDF-2C4A-9395-9C2488F9E4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
made some updates, modified colors && driver.py
</commit_message>
<xml_diff>
--- a/src/crsr_data/CRSRTrackingGrid.xlsx
+++ b/src/crsr_data/CRSRTrackingGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/src/crsr_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C148D7EB-9E05-FB4D-B46B-16EC7C26F984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A29750-4240-F643-B976-D5E505C13972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" activeTab="1" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
   <sheets>
     <sheet name="CRSRShares" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A445721-F1D6-914D-B3EC-B544700EEF22}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -546,9 +546,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5CCD2D-3D10-9346-8A5C-475560897FB9}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -604,7 +604,7 @@
         <v>106</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
         <v>124</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -660,6 +660,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>62</v>
+      </c>
+      <c r="B14" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
crsr shares / covered calls
</commit_message>
<xml_diff>
--- a/src/crsr_data/CRSRTrackingGrid.xlsx
+++ b/src/crsr_data/CRSRTrackingGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/src/crsr_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352AD2B4-1F9F-1142-8F55-99163CC2FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0EE15-2137-2745-95BA-BBD20C7F2022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" activeTab="1" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
   <sheets>
     <sheet name="CRSRShares" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A445721-F1D6-914D-B3EC-B544700EEF22}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,6 +539,14 @@
         <v>26.36</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>29.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -548,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5CCD2D-3D10-9346-8A5C-475560897FB9}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +644,7 @@
         <v>136</v>
       </c>
       <c r="B10" s="5">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
making last push -- leaving CRSR
</commit_message>
<xml_diff>
--- a/src/crsr_data/CRSRTrackingGrid.xlsx
+++ b/src/crsr_data/CRSRTrackingGrid.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/src/crsr_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0EE15-2137-2745-95BA-BBD20C7F2022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B00C8-B6AF-3442-BB3D-409CD7A1C613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" activeTab="1" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
   <sheets>
     <sheet name="CRSRShares" sheetId="1" r:id="rId1"/>
     <sheet name="CRSRCoveredCalls" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -422,11 +422,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A445721-F1D6-914D-B3EC-B544700EEF22}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
@@ -554,13 +554,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5CCD2D-3D10-9346-8A5C-475560897FB9}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.83203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="25" style="5" customWidth="1"/>
@@ -652,7 +652,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="5">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -676,7 +676,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="5">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -684,6 +684,14 @@
         <v>56</v>
       </c>
       <c r="B15" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding TODO comments -- final update for excel doc
</commit_message>
<xml_diff>
--- a/src/crsr_data/CRSRTrackingGrid.xlsx
+++ b/src/crsr_data/CRSRTrackingGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/src/crsr_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B00C8-B6AF-3442-BB3D-409CD7A1C613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B1898D-8BB6-9746-844B-3B37869DA397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="12660" activeTab="1" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>